<commit_message>
1.added reports 2.added reports
</commit_message>
<xml_diff>
--- a/CBS2/test-data/UserAndRoles.xlsx
+++ b/CBS2/test-data/UserAndRoles.xlsx
@@ -4161,9 +4161,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="40">
@@ -4289,6 +4289,35 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -4300,16 +4329,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -4323,29 +4353,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -4355,51 +4362,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4421,6 +4384,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -4430,10 +4408,32 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -4482,13 +4482,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4500,7 +4512,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4512,61 +4644,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4578,91 +4656,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4729,6 +4729,15 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4"/>
       </bottom>
@@ -4750,32 +4759,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4795,22 +4785,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4823,153 +4808,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="22" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="27" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="27" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -52460,11 +52460,14 @@
   <sheetPr/>
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1"/>
+  <cols>
+    <col min="29" max="29" width="11.7142857142857"/>
+  </cols>
   <sheetData>
     <row r="1" ht="38.25" spans="1:32">
       <c r="A1" s="23" t="s">
@@ -52650,7 +52653,7 @@
         <v>117</v>
       </c>
       <c r="AC2" s="15">
-        <v>9122900031</v>
+        <v>7903181938</v>
       </c>
       <c r="AD2" s="15" t="s">
         <v>1278</v>

</xml_diff>